<commit_message>
Nettoyage des base de données
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,6 +8,9 @@
   <sheets>
     <sheet name="Total WYCC" r:id="rId3" sheetId="1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Total">'Total WYCC'!A1:A1</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -14734,7 +14737,7 @@
         </is>
       </c>
       <c r="K5" s="458" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L5" s="458" t="n">
         <v>42643.0</v>
@@ -15252,7 +15255,7 @@
         </is>
       </c>
       <c r="K6" s="571" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L6" s="571" t="n">
         <v>42735.0</v>
@@ -15770,7 +15773,7 @@
         </is>
       </c>
       <c r="K7" s="684" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L7" s="684" t="n">
         <v>42886.0</v>
@@ -16288,7 +16291,7 @@
         </is>
       </c>
       <c r="K8" s="797" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L8" s="797" t="n">
         <v>42663.0</v>
@@ -16806,7 +16809,7 @@
         </is>
       </c>
       <c r="K9" s="910" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L9" s="910" t="n">
         <v>42886.0</v>
@@ -17324,7 +17327,7 @@
         </is>
       </c>
       <c r="K10" s="1023" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L10" s="1023" t="n">
         <v>42553.0</v>
@@ -17842,7 +17845,7 @@
         </is>
       </c>
       <c r="K11" s="1136" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L11" s="1136" t="n">
         <v>42886.0</v>
@@ -18360,7 +18363,7 @@
         </is>
       </c>
       <c r="K12" s="1249" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L12" s="1249" t="n">
         <v>42674.0</v>
@@ -18878,7 +18881,7 @@
         </is>
       </c>
       <c r="K13" s="1362" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L13" s="1362" t="n">
         <v>42886.0</v>
@@ -19396,7 +19399,7 @@
         </is>
       </c>
       <c r="K14" s="1475" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L14" s="1475" t="n">
         <v>42643.0</v>
@@ -19914,7 +19917,7 @@
         </is>
       </c>
       <c r="K15" s="1588" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L15" s="1588" t="n">
         <v>42643.0</v>
@@ -20432,7 +20435,7 @@
         </is>
       </c>
       <c r="K16" s="1701" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L16" s="1701" t="n">
         <v>42663.0</v>
@@ -20719,7 +20722,7 @@
         </is>
       </c>
       <c r="K17" s="1759" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L17" s="1759" t="n">
         <v>42776.0</v>
@@ -21237,7 +21240,7 @@
         </is>
       </c>
       <c r="K18" s="1872" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L18" s="1872" t="n">
         <v>42886.0</v>
@@ -21755,7 +21758,7 @@
         </is>
       </c>
       <c r="K19" s="1985" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L19" s="1985" t="n">
         <v>42886.0</v>
@@ -23827,7 +23830,7 @@
         </is>
       </c>
       <c r="K23" s="2437" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L23" s="2437" t="n">
         <v>42886.0</v>
@@ -24345,7 +24348,7 @@
         </is>
       </c>
       <c r="K24" s="2550" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L24" s="2550" t="n">
         <v>42643.0</v>
@@ -24863,7 +24866,7 @@
         </is>
       </c>
       <c r="K25" s="2663" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L25" s="2663" t="n">
         <v>42735.0</v>
@@ -25381,7 +25384,7 @@
         </is>
       </c>
       <c r="K26" s="2776" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L26" s="2776" t="n">
         <v>42886.0</v>
@@ -25899,7 +25902,7 @@
         </is>
       </c>
       <c r="K27" s="2889" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L27" s="2889" t="n">
         <v>42766.0</v>
@@ -27971,7 +27974,7 @@
         </is>
       </c>
       <c r="K31" s="3341" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L31" s="3341" t="n">
         <v>42735.0</v>
@@ -28489,7 +28492,7 @@
         </is>
       </c>
       <c r="K32" s="3454" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L32" s="3454" t="n">
         <v>42886.0</v>
@@ -29007,7 +29010,7 @@
         </is>
       </c>
       <c r="K33" s="3567" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L33" s="3567" t="n">
         <v>42735.0</v>
@@ -29525,7 +29528,7 @@
         </is>
       </c>
       <c r="K34" s="3680" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L34" s="3680" t="n">
         <v>42825.0</v>
@@ -30561,7 +30564,7 @@
         </is>
       </c>
       <c r="K36" s="3906" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L36" s="3906" t="n">
         <v>42643.0</v>
@@ -31079,7 +31082,7 @@
         </is>
       </c>
       <c r="K37" s="4019" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L37" s="4019" t="n">
         <v>42662.0</v>
@@ -32115,7 +32118,7 @@
         </is>
       </c>
       <c r="K39" s="4245" t="n">
-        <v>42736.998460648145</v>
+        <v>42736.913935185185</v>
       </c>
       <c r="L39" s="4245" t="n">
         <v>42816.0</v>

</xml_diff>